<commit_message>
cambos visuales formilario inventario
</commit_message>
<xml_diff>
--- a/Portal/templates/templatesDocs/Inventario Oficina.xlsx
+++ b/Portal/templates/templatesDocs/Inventario Oficina.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeihb\Desktop\CrudIn\Portal\templates\templatesDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739B5707-AA28-4986-A84A-73CB107408B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B171B69-B2FC-4578-9B63-3DD11255BD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="2625" windowWidth="21600" windowHeight="11295" xr2:uid="{E6A4F7F0-F9E9-47BA-8663-D0C27572CA8E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6A4F7F0-F9E9-47BA-8663-D0C27572CA8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,19 +119,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFF3CD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor rgb="FFFFE8A1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,23 +168,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -200,6 +200,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFE8A1"/>
+      <color rgb="FFFFF3CD"/>
       <color rgb="FFFFCC00"/>
     </mruColors>
   </colors>
@@ -534,7 +536,7 @@
   <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,134 +573,134 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="4">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
+      <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="B9" s="10">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="B11" s="10">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>

</xml_diff>